<commit_message>
Currently available list of components detail
</commit_message>
<xml_diff>
--- a/Available_Component_List.xlsx
+++ b/Available_Component_List.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OvenProject\Oven_Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Oven_Git\07-10 - Doc\Oven_Documentations\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="33">
   <si>
     <t>Component</t>
   </si>
@@ -41,21 +41,6 @@
     <t xml:space="preserve">MCP3008 </t>
   </si>
   <si>
-    <t>7 pics</t>
-  </si>
-  <si>
-    <t>9 pics</t>
-  </si>
-  <si>
-    <t>6 pics</t>
-  </si>
-  <si>
-    <t>2 pics</t>
-  </si>
-  <si>
-    <t>1 pics</t>
-  </si>
-  <si>
     <t>Bluetooth Module</t>
   </si>
   <si>
@@ -74,15 +59,6 @@
     <t xml:space="preserve">speaker wire </t>
   </si>
   <si>
-    <t>3 pics</t>
-  </si>
-  <si>
-    <t>9 Pics</t>
-  </si>
-  <si>
-    <t>17 pics</t>
-  </si>
-  <si>
     <t xml:space="preserve">Audio jack Cable </t>
   </si>
   <si>
@@ -107,20 +83,53 @@
     <t>3 pin RMC Cable</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>Verification</t>
   </si>
   <si>
     <t>ok</t>
+  </si>
+  <si>
+    <t>4 No's</t>
+  </si>
+  <si>
+    <t>2 No's</t>
+  </si>
+  <si>
+    <t>3 No's</t>
+  </si>
+  <si>
+    <t>5 No's</t>
+  </si>
+  <si>
+    <t>3 pin Jst Cable</t>
+  </si>
+  <si>
+    <t>1 No</t>
+  </si>
+  <si>
+    <t>0 No</t>
+  </si>
+  <si>
+    <t>10 No's</t>
+  </si>
+  <si>
+    <t>12 No's</t>
+  </si>
+  <si>
+    <t>3 Pin Plug &amp; Socket</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bolts </t>
+  </si>
+  <si>
+    <t>CT Coils</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -128,13 +137,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -164,16 +187,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -455,28 +485,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D22"/>
+  <dimension ref="B2:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="29.26953125" customWidth="1"/>
     <col min="3" max="3" width="19.81640625" customWidth="1"/>
-    <col min="4" max="4" width="10.54296875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="10.54296875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>28</v>
+      <c r="D2" s="6" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="2:4" ht="5.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -485,203 +515,248 @@
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B6" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" ht="4.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="4"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B15" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="C15" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B16" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" ht="5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="4"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="2:4" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B7" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B8" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="1" t="s">
+      <c r="D19" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B20" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B21" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B9" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B12" s="2" t="s">
+      <c r="C21" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B22" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" ht="4.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="2"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B14" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B15" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B16" s="2" t="s">
+      <c r="C23" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" ht="5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="2"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B18" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B19" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B20" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B21" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B22" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>29</v>
+      <c r="D26" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>